<commit_message>
Updating the tide-wind paper2-3 cases
</commit_message>
<xml_diff>
--- a/TideWindNew/Parameters.xlsx
+++ b/TideWindNew/Parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHUb\suntans\TideWindNew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A85834D-7F8C-4ADC-9D67-84793CF98769}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6621B1F-5093-412A-B39E-2E654E35A7D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19196" xr2:uid="{211BB758-569C-40AC-9BC8-2D9CA9893642}"/>
   </bookViews>
@@ -912,9 +912,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAADB4C0-B9DD-42B5-A85A-4458C7550D84}">
   <dimension ref="A1:P504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A463" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A448" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B507" sqref="B507"/>
+      <selection pane="topRight" activeCell="A467" sqref="A467:XFD467"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>